<commit_message>
chl, ppd, phyto size class, wcr
</commit_message>
<xml_diff>
--- a/data-raw/WCR.xlsx
+++ b/data-raw/WCR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimberly.bastille\Desktop\Rgghhh\ecodata2020\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimberly.bastille\Desktop\Rgghhh\ecodata\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -389,9 +389,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -723,6 +725,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2021</v>
+      </c>
+      <c r="C42">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
minor edits from Synthesis meeting
</commit_message>
<xml_diff>
--- a/data-raw/WCR.xlsx
+++ b/data-raw/WCR.xlsx
@@ -389,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,14 +725,6 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>2021</v>
-      </c>
-      <c r="C42">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>